<commit_message>
Duplicate Analysis and Reference Sample for LactoScope
</commit_message>
<xml_diff>
--- a/src/senaite/instruments/tests/files/instruments/perkinelmer/lactoscope/Lactoscope_H230613_16COMP.xlsx
+++ b/src/senaite/instruments/tests/files/instruments/perkinelmer/lactoscope/Lactoscope_H230613_16COMP.xlsx
@@ -114,6 +114,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -135,6 +136,7 @@
       <color rgb="FF434343"/>
       <name val="Open Sans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -335,10 +337,10 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.57"/>

</xml_diff>